<commit_message>
sig points plot created
</commit_message>
<xml_diff>
--- a/Lab 12/Problem 1.xlsx
+++ b/Lab 12/Problem 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pearl\Desktop\Edumacation\ATSC 303\Lab 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC245EDF-69CF-4FDD-BBF2-E047EF20AE30}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5795DBDA-3101-44B1-99AA-22D498D08A51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>T significant points</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Lon (degN)</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
@@ -828,10 +831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FA0A38-7381-4D8C-A322-E2EF3CC535BA}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3:M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -884,1068 +887,2426 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>8326</v>
+        <v>498</v>
       </c>
       <c r="B3">
-        <v>53.5</v>
+        <v>850.2</v>
       </c>
       <c r="C3">
-        <v>20045</v>
+        <v>1399</v>
       </c>
       <c r="D3">
-        <v>-50.15</v>
+        <v>-1.75</v>
       </c>
       <c r="E3">
-        <v>-83.85</v>
+        <v>-11.55</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="G3">
-        <v>2.85</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="H3">
-        <v>-3.46</v>
+        <v>-7.39</v>
       </c>
       <c r="I3">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J3">
-        <v>4.5</v>
+        <v>8.5</v>
       </c>
       <c r="K3">
-        <v>16.2</v>
+        <v>30.6</v>
       </c>
       <c r="L3">
-        <v>-123.01</v>
+        <v>-123.28</v>
       </c>
       <c r="M3">
-        <v>49.76</v>
+        <v>49.26</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>7604</v>
+        <v>262</v>
       </c>
       <c r="B4">
-        <v>71.7</v>
+        <v>916.4</v>
       </c>
       <c r="C4">
-        <v>18153</v>
+        <v>797</v>
       </c>
       <c r="D4">
-        <v>-54.35</v>
+        <v>3.3500000000000201</v>
       </c>
       <c r="E4">
-        <v>-86.85</v>
+        <v>-11.05</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="G4">
-        <v>6.81</v>
+        <v>0.72</v>
       </c>
       <c r="H4">
-        <v>1.45</v>
+        <v>-8.9600000000000009</v>
       </c>
       <c r="I4">
-        <v>192</v>
+        <v>95</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K4">
-        <v>25.2</v>
+        <v>32.4</v>
       </c>
       <c r="L4">
-        <v>-123.03</v>
+        <v>-123.25</v>
       </c>
       <c r="M4">
-        <v>49.74</v>
+        <v>49.25</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>6942</v>
+        <v>8578</v>
       </c>
       <c r="B5">
-        <v>94.7</v>
+        <v>48.1</v>
       </c>
       <c r="C5">
-        <v>16365</v>
+        <v>20746</v>
       </c>
       <c r="D5">
-        <v>-50.45</v>
+        <v>-52.15</v>
       </c>
       <c r="E5">
-        <v>-84.05</v>
+        <v>-85.25</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>10.69</v>
+        <v>3.32</v>
       </c>
       <c r="H5">
-        <v>3.78</v>
+        <v>-5.92</v>
       </c>
       <c r="I5">
-        <v>199</v>
+        <v>119</v>
       </c>
       <c r="J5">
-        <v>11.3</v>
+        <v>6.8</v>
       </c>
       <c r="K5">
-        <v>40.68</v>
+        <v>24.48</v>
       </c>
       <c r="L5">
-        <v>-123.06</v>
+        <v>-123.02</v>
       </c>
       <c r="M5">
-        <v>49.71</v>
+        <v>49.76</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>6260</v>
+        <v>8364</v>
       </c>
       <c r="B6">
-        <v>124.7</v>
+        <v>52.8</v>
       </c>
       <c r="C6">
-        <v>14573</v>
+        <v>20139</v>
       </c>
       <c r="D6">
-        <v>-51.75</v>
+        <v>-50.35</v>
       </c>
       <c r="E6">
-        <v>-85.05</v>
+        <v>-84.05</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>9.2200000000000006</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H6">
-        <v>0.81</v>
+        <v>-4.57</v>
       </c>
       <c r="I6">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="J6">
-        <v>9.3000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="K6">
-        <v>33.479999999999997</v>
+        <v>23.4</v>
       </c>
       <c r="L6">
-        <v>-123.09</v>
+        <v>-123.01</v>
       </c>
       <c r="M6">
-        <v>49.67</v>
+        <v>49.76</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>5810</v>
+        <v>7602</v>
       </c>
       <c r="B7">
-        <v>149.6</v>
+        <v>71.8</v>
       </c>
       <c r="C7">
-        <v>13384</v>
+        <v>18148</v>
       </c>
       <c r="D7">
-        <v>-48.15</v>
+        <v>-54.45</v>
       </c>
       <c r="E7">
-        <v>-82.45</v>
+        <v>-86.95</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>9.59</v>
+        <v>6.85</v>
       </c>
       <c r="H7">
-        <v>3.53</v>
+        <v>1.38</v>
       </c>
       <c r="I7">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="J7">
-        <v>10.199999999999999</v>
+        <v>7</v>
       </c>
       <c r="K7">
-        <v>36.72</v>
+        <v>25.2</v>
       </c>
       <c r="L7">
-        <v>-123.1</v>
+        <v>-123.03</v>
       </c>
       <c r="M7">
-        <v>49.64</v>
+        <v>49.74</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>4890</v>
+        <v>6940</v>
       </c>
       <c r="B8">
-        <v>210.6</v>
+        <v>94.7</v>
       </c>
       <c r="C8">
-        <v>11142</v>
+        <v>16360</v>
       </c>
       <c r="D8">
-        <v>-50.75</v>
+        <v>-50.45</v>
       </c>
       <c r="E8">
-        <v>-84.35</v>
+        <v>-84.05</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8">
-        <v>9.81</v>
+        <v>10.71</v>
       </c>
       <c r="H8">
-        <v>0.66</v>
+        <v>3.67</v>
       </c>
       <c r="I8">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="J8">
-        <v>9.8000000000000007</v>
+        <v>11.3</v>
       </c>
       <c r="K8">
-        <v>35.28</v>
+        <v>40.68</v>
       </c>
       <c r="L8">
-        <v>-123.12</v>
+        <v>-123.06</v>
       </c>
       <c r="M8">
-        <v>49.57</v>
+        <v>49.71</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>4170</v>
+        <v>6220</v>
       </c>
       <c r="B9">
-        <v>274.5</v>
+        <v>126.6</v>
       </c>
       <c r="C9">
-        <v>9433</v>
+        <v>14472</v>
       </c>
       <c r="D9">
-        <v>-54.65</v>
+        <v>-51.65</v>
       </c>
       <c r="E9">
-        <v>-67.650000000000006</v>
+        <v>-84.95</v>
       </c>
       <c r="F9">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>8.98</v>
+        <v>9.68</v>
       </c>
       <c r="H9">
-        <v>5.56</v>
+        <v>0.61</v>
       </c>
       <c r="I9">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="J9">
-        <v>10.6</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="K9">
-        <v>38.159999999999997</v>
+        <v>34.92</v>
       </c>
       <c r="L9">
-        <v>-123.13</v>
+        <v>-123.09</v>
       </c>
       <c r="M9">
-        <v>49.51</v>
+        <v>49.67</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>4138</v>
+        <v>5814</v>
       </c>
       <c r="B10">
-        <v>277.60000000000002</v>
+        <v>149.4</v>
       </c>
       <c r="C10">
-        <v>9362</v>
+        <v>13394</v>
       </c>
       <c r="D10">
-        <v>-55.45</v>
+        <v>-48.15</v>
       </c>
       <c r="E10">
-        <v>-69.75</v>
+        <v>-82.45</v>
       </c>
       <c r="F10">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>10.07</v>
+        <v>9.52</v>
       </c>
       <c r="H10">
-        <v>7.11</v>
+        <v>3.61</v>
       </c>
       <c r="I10">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="J10">
-        <v>12.3</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="K10">
-        <v>44.28</v>
+        <v>36.72</v>
       </c>
       <c r="L10">
-        <v>-123.13</v>
+        <v>-123.1</v>
       </c>
       <c r="M10">
-        <v>49.51</v>
+        <v>49.64</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>2922</v>
+        <v>4856</v>
       </c>
       <c r="B11">
-        <v>420.9</v>
+        <v>213.2</v>
       </c>
       <c r="C11">
-        <v>6620</v>
+        <v>11062</v>
       </c>
       <c r="D11">
-        <v>-37.450000000000003</v>
+        <v>-50.55</v>
       </c>
       <c r="E11">
-        <v>-45.15</v>
+        <v>-84.05</v>
       </c>
       <c r="F11">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>6.21</v>
+        <v>8.64</v>
       </c>
       <c r="H11">
-        <v>3.61</v>
+        <v>0.41</v>
       </c>
       <c r="I11">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="J11">
-        <v>7.2</v>
+        <v>8.6</v>
       </c>
       <c r="K11">
-        <v>25.92</v>
+        <v>30.96</v>
       </c>
       <c r="L11">
-        <v>-123.21</v>
+        <v>-123.12</v>
       </c>
       <c r="M11">
-        <v>49.41</v>
+        <v>49.57</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>2544</v>
+        <v>4720</v>
       </c>
       <c r="B12">
-        <v>474.5</v>
+        <v>224.4</v>
       </c>
       <c r="C12">
-        <v>5780</v>
+        <v>10728</v>
       </c>
       <c r="D12">
-        <v>-30.75</v>
+        <v>-51.95</v>
       </c>
       <c r="E12">
-        <v>-55.65</v>
+        <v>-80.650000000000006</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>7.28</v>
+        <v>10.64</v>
       </c>
       <c r="H12">
-        <v>3.55</v>
+        <v>-0.2</v>
       </c>
       <c r="I12">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="J12">
-        <v>8.1</v>
+        <v>10.6</v>
       </c>
       <c r="K12">
-        <v>29.16</v>
+        <v>38.159999999999997</v>
       </c>
       <c r="L12">
-        <v>-123.22</v>
+        <v>-123.12</v>
       </c>
       <c r="M12">
-        <v>49.39</v>
+        <v>49.56</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>2470</v>
+        <v>4592</v>
       </c>
       <c r="B13">
-        <v>485</v>
+        <v>234.9</v>
       </c>
       <c r="C13">
-        <v>5624</v>
+        <v>10434</v>
       </c>
       <c r="D13">
-        <v>-29.55</v>
+        <v>-52.85</v>
       </c>
       <c r="E13">
-        <v>-46.15</v>
+        <v>-81.150000000000006</v>
       </c>
       <c r="F13">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>6.72</v>
+        <v>8.82</v>
       </c>
       <c r="H13">
-        <v>4.87</v>
+        <v>0.63</v>
       </c>
       <c r="I13">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="J13">
-        <v>8.3000000000000007</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="K13">
-        <v>29.88</v>
+        <v>31.68</v>
       </c>
       <c r="L13">
-        <v>-123.23</v>
+        <v>-123.12</v>
       </c>
       <c r="M13">
-        <v>49.39</v>
+        <v>49.55</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>2444</v>
+        <v>4270</v>
       </c>
       <c r="B14">
-        <v>488.8</v>
+        <v>265.10000000000002</v>
       </c>
       <c r="C14">
-        <v>5569</v>
+        <v>9655</v>
       </c>
       <c r="D14">
-        <v>-29.35</v>
+        <v>-53.85</v>
       </c>
       <c r="E14">
-        <v>-50.95</v>
+        <v>-76.650000000000006</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G14">
-        <v>6.33</v>
+        <v>9.34</v>
       </c>
       <c r="H14">
-        <v>5.27</v>
+        <v>-1.26</v>
       </c>
       <c r="I14">
-        <v>220</v>
+        <v>172</v>
       </c>
       <c r="J14">
-        <v>8.1999999999999993</v>
+        <v>9.4</v>
       </c>
       <c r="K14">
-        <v>29.52</v>
+        <v>33.840000000000003</v>
       </c>
       <c r="L14">
-        <v>-123.23</v>
+        <v>-123.13</v>
       </c>
       <c r="M14">
-        <v>49.38</v>
+        <v>49.52</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>2378</v>
+        <v>4170</v>
       </c>
       <c r="B15">
-        <v>498.4</v>
+        <v>274.5</v>
       </c>
       <c r="C15">
-        <v>5429</v>
+        <v>9433</v>
       </c>
       <c r="D15">
-        <v>-28.85</v>
+        <v>-54.65</v>
       </c>
       <c r="E15">
-        <v>-45.95</v>
+        <v>-67.650000000000006</v>
       </c>
       <c r="F15">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15">
-        <v>4.92</v>
+        <v>8.98</v>
       </c>
       <c r="H15">
-        <v>5.89</v>
+        <v>5.56</v>
       </c>
       <c r="I15">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="J15">
-        <v>7.7</v>
+        <v>10.6</v>
       </c>
       <c r="K15">
-        <v>27.72</v>
+        <v>38.159999999999997</v>
       </c>
       <c r="L15">
-        <v>-123.23</v>
+        <v>-123.13</v>
       </c>
       <c r="M15">
-        <v>49.38</v>
+        <v>49.51</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>2306</v>
+        <v>4106</v>
       </c>
       <c r="B16">
-        <v>509.2</v>
+        <v>280.8</v>
       </c>
       <c r="C16">
-        <v>5276</v>
+        <v>9288</v>
       </c>
       <c r="D16">
-        <v>-27.75</v>
+        <v>-55.15</v>
       </c>
       <c r="E16">
-        <v>-52.85</v>
+        <v>-66.849999999999994</v>
       </c>
       <c r="F16">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="G16">
-        <v>4.96</v>
+        <v>10.18</v>
       </c>
       <c r="H16">
-        <v>5.98</v>
+        <v>7.4</v>
       </c>
       <c r="I16">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="J16">
-        <v>7.8</v>
+        <v>12.6</v>
       </c>
       <c r="K16">
-        <v>28.08</v>
+        <v>45.36</v>
       </c>
       <c r="L16">
-        <v>-123.24</v>
+        <v>-123.14</v>
       </c>
       <c r="M16">
-        <v>49.38</v>
+        <v>49.51</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>2160</v>
+        <v>4056</v>
       </c>
       <c r="B17">
-        <v>531.79999999999995</v>
+        <v>285.89999999999998</v>
       </c>
       <c r="C17">
-        <v>4964</v>
+        <v>9172</v>
       </c>
       <c r="D17">
-        <v>-27.75</v>
+        <v>-54.85</v>
       </c>
       <c r="E17">
-        <v>-29.85</v>
+        <v>-65.75</v>
       </c>
       <c r="F17">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="G17">
-        <v>7.64</v>
+        <v>10.23</v>
       </c>
       <c r="H17">
-        <v>9.61</v>
+        <v>8.6</v>
       </c>
       <c r="I17">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="J17">
-        <v>12.3</v>
+        <v>13.4</v>
       </c>
       <c r="K17">
-        <v>44.28</v>
+        <v>48.24</v>
       </c>
       <c r="L17">
-        <v>-123.25</v>
+        <v>-123.14</v>
       </c>
       <c r="M17">
-        <v>49.37</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>886</v>
+        <v>4014</v>
       </c>
       <c r="B18">
-        <v>765.6</v>
+        <v>290.39999999999998</v>
       </c>
       <c r="C18">
-        <v>2225</v>
+        <v>9073</v>
       </c>
       <c r="D18">
-        <v>-6.5499999999999501</v>
+        <v>-54.65</v>
       </c>
       <c r="E18">
-        <v>-9.4499999999999904</v>
+        <v>-71.45</v>
       </c>
       <c r="F18">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="G18">
-        <v>8.39</v>
+        <v>11.16</v>
       </c>
       <c r="H18">
-        <v>-2.77</v>
+        <v>8.51</v>
       </c>
       <c r="I18">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="J18">
-        <v>8.8000000000000007</v>
+        <v>14</v>
       </c>
       <c r="K18">
-        <v>31.68</v>
+        <v>50.4</v>
       </c>
       <c r="L18">
-        <v>-123.31</v>
+        <v>-123.15</v>
       </c>
       <c r="M18">
-        <v>49.28</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>818</v>
+        <v>3604</v>
       </c>
       <c r="B19">
-        <v>780.6</v>
+        <v>336.2</v>
       </c>
       <c r="C19">
-        <v>2073</v>
+        <v>8128</v>
       </c>
       <c r="D19">
-        <v>-5.5499999999999501</v>
+        <v>-50.15</v>
       </c>
       <c r="E19">
-        <v>-12.05</v>
+        <v>-56.15</v>
       </c>
       <c r="F19">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G19">
-        <v>10.61</v>
+        <v>7.39</v>
       </c>
       <c r="H19">
-        <v>-3.38</v>
+        <v>3.46</v>
       </c>
       <c r="I19">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="J19">
-        <v>11.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="K19">
-        <v>39.96</v>
+        <v>29.52</v>
       </c>
       <c r="L19">
-        <v>-123.3</v>
+        <v>-123.18</v>
       </c>
       <c r="M19">
-        <v>49.28</v>
+        <v>49.46</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>392</v>
+        <v>3452</v>
       </c>
       <c r="B20">
-        <v>875.4</v>
+        <v>356.4</v>
       </c>
       <c r="C20">
-        <v>1165</v>
+        <v>7743</v>
       </c>
       <c r="D20">
-        <v>0.25</v>
+        <v>-46.45</v>
       </c>
       <c r="E20">
-        <v>-13.65</v>
+        <v>-55.55</v>
       </c>
       <c r="F20">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G20">
-        <v>3.15</v>
+        <v>8.31</v>
       </c>
       <c r="H20">
-        <v>-7.93</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="I20">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="J20">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="K20">
-        <v>30.6</v>
+        <v>30.96</v>
       </c>
       <c r="L20">
-        <v>-123.27</v>
+        <v>-123.18</v>
       </c>
       <c r="M20">
-        <v>49.25</v>
+        <v>49.45</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>666</v>
+        <v>3262</v>
       </c>
       <c r="B21">
-        <v>812.3</v>
+        <v>378.1</v>
       </c>
       <c r="C21">
-        <v>1760</v>
+        <v>7350</v>
       </c>
       <c r="D21">
-        <v>-4.0499999999999501</v>
+        <v>-43.65</v>
       </c>
       <c r="E21">
-        <v>-8.1499999999999808</v>
+        <v>-50.15</v>
       </c>
       <c r="F21">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="G21">
-        <v>6.89</v>
+        <v>8.75</v>
       </c>
       <c r="H21">
-        <v>-6.05</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="I21">
-        <v>139</v>
+        <v>205</v>
       </c>
       <c r="J21">
-        <v>9.1999999999999993</v>
+        <v>9.6</v>
       </c>
       <c r="K21">
-        <v>33.119999999999997</v>
+        <v>34.56</v>
       </c>
       <c r="L21">
-        <v>-123.29</v>
+        <v>-123.19</v>
       </c>
       <c r="M21">
-        <v>49.27</v>
+        <v>49.43</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>162</v>
+        <v>3044</v>
       </c>
       <c r="B22">
-        <v>946.5</v>
+        <v>404.2</v>
       </c>
       <c r="C22">
-        <v>534</v>
+        <v>6897</v>
       </c>
       <c r="D22">
-        <v>5.0500000000000096</v>
+        <v>-39.75</v>
       </c>
       <c r="E22">
-        <v>-7.4499999999999904</v>
+        <v>-47.95</v>
       </c>
       <c r="F22">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G22">
-        <v>-0.97</v>
+        <v>7.5</v>
       </c>
       <c r="H22">
-        <v>-4.6399999999999997</v>
+        <v>3.68</v>
       </c>
       <c r="I22">
-        <v>78</v>
+        <v>206</v>
       </c>
       <c r="J22">
-        <v>4.7</v>
+        <v>8.4</v>
       </c>
       <c r="K22">
-        <v>16.920000000000002</v>
+        <v>30.24</v>
       </c>
       <c r="L22">
-        <v>-123.24</v>
+        <v>-123.2</v>
       </c>
       <c r="M22">
-        <v>49.25</v>
+        <v>49.42</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>140</v>
+        <v>3014</v>
       </c>
       <c r="B23">
-        <v>951.4</v>
+        <v>408.2</v>
       </c>
       <c r="C23">
-        <v>492</v>
+        <v>6829</v>
       </c>
       <c r="D23">
-        <v>3.6500000000000301</v>
+        <v>-39.15</v>
       </c>
       <c r="E23">
-        <v>-2.3499999999999699</v>
+        <v>-50.35</v>
       </c>
       <c r="F23">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="G23">
-        <v>-1.18</v>
+        <v>6.75</v>
       </c>
       <c r="H23">
-        <v>-3.68</v>
+        <v>3.64</v>
       </c>
       <c r="I23">
-        <v>72</v>
+        <v>208</v>
       </c>
       <c r="J23">
-        <v>3.9</v>
+        <v>7.7</v>
       </c>
       <c r="K23">
-        <v>14.04</v>
+        <v>27.72</v>
       </c>
       <c r="L23">
-        <v>-123.24</v>
+        <v>-123.2</v>
       </c>
       <c r="M23">
-        <v>49.25</v>
+        <v>49.42</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>4</v>
+        <v>2920</v>
       </c>
       <c r="B24">
-        <v>998.3</v>
+        <v>421.1</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>6615</v>
       </c>
       <c r="D24">
-        <v>4.8500000000000201</v>
+        <v>-37.450000000000003</v>
       </c>
       <c r="E24">
-        <v>-1.25</v>
+        <v>-45.25</v>
       </c>
       <c r="F24">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G24">
-        <v>1.56</v>
+        <v>6.2</v>
       </c>
       <c r="H24">
-        <v>1.38</v>
+        <v>3.6</v>
       </c>
       <c r="I24">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="J24">
-        <v>2.1</v>
+        <v>7.2</v>
       </c>
       <c r="K24">
-        <v>7.56</v>
+        <v>25.92</v>
       </c>
       <c r="L24">
-        <v>-123.24</v>
+        <v>-123.21</v>
       </c>
       <c r="M24">
-        <v>49.25</v>
+        <v>49.41</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>4086</v>
+        <v>2832</v>
       </c>
       <c r="B25">
-        <v>282.8</v>
+        <v>433.7</v>
       </c>
       <c r="C25">
-        <v>9241</v>
+        <v>6412</v>
       </c>
       <c r="D25">
-        <v>-55.15</v>
+        <v>-35.75</v>
       </c>
       <c r="E25">
-        <v>-67.75</v>
+        <v>-44.85</v>
       </c>
       <c r="F25">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G25">
-        <v>10.09</v>
+        <v>5.55</v>
       </c>
       <c r="H25">
-        <v>7.97</v>
+        <v>3.07</v>
       </c>
       <c r="I25">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="J25">
-        <v>12.9</v>
+        <v>6.3</v>
       </c>
       <c r="K25">
-        <v>46.44</v>
+        <v>22.68</v>
       </c>
       <c r="L25">
-        <v>-123.14</v>
+        <v>-123.21</v>
       </c>
       <c r="M25">
-        <v>49.51</v>
+        <v>49.41</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>4058</v>
+        <v>2548</v>
       </c>
       <c r="B26">
-        <v>285.7</v>
+        <v>473.9</v>
       </c>
       <c r="C26">
-        <v>9177</v>
+        <v>5788</v>
       </c>
       <c r="D26">
-        <v>-54.85</v>
+        <v>-30.85</v>
       </c>
       <c r="E26">
-        <v>-65.650000000000006</v>
+        <v>-55.55</v>
       </c>
       <c r="F26">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="G26">
-        <v>10.18</v>
+        <v>7.29</v>
       </c>
       <c r="H26">
-        <v>8.57</v>
+        <v>3.36</v>
       </c>
       <c r="I26">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="J26">
-        <v>13.3</v>
+        <v>8</v>
       </c>
       <c r="K26">
-        <v>47.88</v>
+        <v>28.8</v>
       </c>
       <c r="L26">
-        <v>-123.14</v>
+        <v>-123.22</v>
       </c>
       <c r="M26">
-        <v>49.5</v>
+        <v>49.39</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>4098</v>
+        <v>2446</v>
       </c>
       <c r="B27">
-        <v>281.60000000000002</v>
+        <v>488.5</v>
       </c>
       <c r="C27">
-        <v>9269</v>
+        <v>5573</v>
       </c>
       <c r="D27">
-        <v>-55.05</v>
+        <v>-29.45</v>
       </c>
       <c r="E27">
-        <v>-66.55</v>
+        <v>-50.75</v>
       </c>
       <c r="F27">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G27">
-        <v>10.16</v>
+        <v>6.34</v>
       </c>
       <c r="H27">
-        <v>7.64</v>
+        <v>5.22</v>
       </c>
       <c r="I27">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J27">
-        <v>12.7</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="K27">
-        <v>45.72</v>
+        <v>29.52</v>
       </c>
       <c r="L27">
-        <v>-123.14</v>
+        <v>-123.23</v>
       </c>
       <c r="M27">
-        <v>49.51</v>
+        <v>49.38</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>3998</v>
+        <v>2468</v>
       </c>
       <c r="B28">
-        <v>292.10000000000002</v>
+        <v>485.3</v>
       </c>
       <c r="C28">
-        <v>9035</v>
+        <v>5620</v>
       </c>
       <c r="D28">
+        <v>-29.55</v>
+      </c>
+      <c r="E28">
+        <v>-46.05</v>
+      </c>
+      <c r="F28">
+        <v>19</v>
+      </c>
+      <c r="G28">
+        <v>6.72</v>
+      </c>
+      <c r="H28">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="I28">
+        <v>216</v>
+      </c>
+      <c r="J28">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K28">
+        <v>29.88</v>
+      </c>
+      <c r="L28">
+        <v>-123.23</v>
+      </c>
+      <c r="M28">
+        <v>49.39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>2388</v>
+      </c>
+      <c r="B29">
+        <v>496.9</v>
+      </c>
+      <c r="C29">
+        <v>5451</v>
+      </c>
+      <c r="D29">
+        <v>-29.05</v>
+      </c>
+      <c r="E29">
+        <v>-46.05</v>
+      </c>
+      <c r="F29">
+        <v>18</v>
+      </c>
+      <c r="G29">
+        <v>5.16</v>
+      </c>
+      <c r="H29">
+        <v>5.9</v>
+      </c>
+      <c r="I29">
+        <v>229</v>
+      </c>
+      <c r="J29">
+        <v>7.8</v>
+      </c>
+      <c r="K29">
+        <v>28.08</v>
+      </c>
+      <c r="L29">
+        <v>-123.23</v>
+      </c>
+      <c r="M29">
+        <v>49.38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>2310</v>
+      </c>
+      <c r="B30">
+        <v>508.6</v>
+      </c>
+      <c r="C30">
+        <v>5284</v>
+      </c>
+      <c r="D30">
+        <v>-27.85</v>
+      </c>
+      <c r="E30">
+        <v>-52.85</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="H30">
+        <v>6.02</v>
+      </c>
+      <c r="I30">
+        <v>231</v>
+      </c>
+      <c r="J30">
+        <v>7.8</v>
+      </c>
+      <c r="K30">
+        <v>28.08</v>
+      </c>
+      <c r="L30">
+        <v>-123.24</v>
+      </c>
+      <c r="M30">
+        <v>49.38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>2150</v>
+      </c>
+      <c r="B31">
+        <v>533.6</v>
+      </c>
+      <c r="C31">
+        <v>4939</v>
+      </c>
+      <c r="D31">
+        <v>-27.65</v>
+      </c>
+      <c r="E31">
+        <v>-29.75</v>
+      </c>
+      <c r="F31">
+        <v>82</v>
+      </c>
+      <c r="G31">
+        <v>7.88</v>
+      </c>
+      <c r="H31">
+        <v>9.57</v>
+      </c>
+      <c r="I31">
+        <v>231</v>
+      </c>
+      <c r="J31">
+        <v>12.4</v>
+      </c>
+      <c r="K31">
+        <v>44.64</v>
+      </c>
+      <c r="L31">
+        <v>-123.26</v>
+      </c>
+      <c r="M31">
+        <v>49.37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>1592</v>
+      </c>
+      <c r="B32">
+        <v>631.70000000000005</v>
+      </c>
+      <c r="C32">
+        <v>3700</v>
+      </c>
+      <c r="D32">
+        <v>-16.95</v>
+      </c>
+      <c r="E32">
+        <v>-22.05</v>
+      </c>
+      <c r="F32">
+        <v>65</v>
+      </c>
+      <c r="G32">
+        <v>6.62</v>
+      </c>
+      <c r="H32">
+        <v>1.55</v>
+      </c>
+      <c r="I32">
+        <v>193</v>
+      </c>
+      <c r="J32">
+        <v>6.8</v>
+      </c>
+      <c r="K32">
+        <v>24.48</v>
+      </c>
+      <c r="L32">
+        <v>-123.3</v>
+      </c>
+      <c r="M32">
+        <v>49.33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>1430</v>
+      </c>
+      <c r="B33">
+        <v>661.2</v>
+      </c>
+      <c r="C33">
+        <v>3355</v>
+      </c>
+      <c r="D33">
+        <v>-13.85</v>
+      </c>
+      <c r="E33">
+        <v>-22.05</v>
+      </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33">
+        <v>6.95</v>
+      </c>
+      <c r="H33">
+        <v>-0.13</v>
+      </c>
+      <c r="I33">
+        <v>179</v>
+      </c>
+      <c r="J33">
+        <v>7</v>
+      </c>
+      <c r="K33">
+        <v>25.2</v>
+      </c>
+      <c r="L33">
+        <v>-123.31</v>
+      </c>
+      <c r="M33">
+        <v>49.32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>1114</v>
+      </c>
+      <c r="B34">
+        <v>718.6</v>
+      </c>
+      <c r="C34">
+        <v>2717</v>
+      </c>
+      <c r="D34">
+        <v>-9.5499999999999599</v>
+      </c>
+      <c r="E34">
+        <v>-12.55</v>
+      </c>
+      <c r="F34">
+        <v>78</v>
+      </c>
+      <c r="G34">
+        <v>7.16</v>
+      </c>
+      <c r="H34">
+        <v>0.69</v>
+      </c>
+      <c r="I34">
+        <v>186</v>
+      </c>
+      <c r="J34">
+        <v>7.2</v>
+      </c>
+      <c r="K34">
+        <v>25.92</v>
+      </c>
+      <c r="L34">
+        <v>-123.31</v>
+      </c>
+      <c r="M34">
+        <v>49.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>1086</v>
+      </c>
+      <c r="B35">
+        <v>724.3</v>
+      </c>
+      <c r="C35">
+        <v>2656</v>
+      </c>
+      <c r="D35">
+        <v>-9.1499999999999808</v>
+      </c>
+      <c r="E35">
+        <v>-13.45</v>
+      </c>
+      <c r="F35">
+        <v>71</v>
+      </c>
+      <c r="G35">
+        <v>7.2</v>
+      </c>
+      <c r="H35">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I35">
+        <v>184</v>
+      </c>
+      <c r="J35">
+        <v>7.2</v>
+      </c>
+      <c r="K35">
+        <v>25.92</v>
+      </c>
+      <c r="L35">
+        <v>-123.31</v>
+      </c>
+      <c r="M35">
+        <v>49.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>880</v>
+      </c>
+      <c r="B36">
+        <v>766.8</v>
+      </c>
+      <c r="C36">
+        <v>2212</v>
+      </c>
+      <c r="D36">
+        <v>-6.5499999999999501</v>
+      </c>
+      <c r="E36">
+        <v>-9.25</v>
+      </c>
+      <c r="F36">
+        <v>81</v>
+      </c>
+      <c r="G36">
+        <v>8.57</v>
+      </c>
+      <c r="H36">
+        <v>-2.89</v>
+      </c>
+      <c r="I36">
+        <v>161</v>
+      </c>
+      <c r="J36">
+        <v>9</v>
+      </c>
+      <c r="K36">
+        <v>32.4</v>
+      </c>
+      <c r="L36">
+        <v>-123.31</v>
+      </c>
+      <c r="M36">
+        <v>49.28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>822</v>
+      </c>
+      <c r="B37">
+        <v>779.8</v>
+      </c>
+      <c r="C37">
+        <v>2081</v>
+      </c>
+      <c r="D37">
+        <v>-5.6499999999999799</v>
+      </c>
+      <c r="E37">
+        <v>-11.95</v>
+      </c>
+      <c r="F37">
+        <v>61</v>
+      </c>
+      <c r="G37">
+        <v>10.57</v>
+      </c>
+      <c r="H37">
+        <v>-3.34</v>
+      </c>
+      <c r="I37">
+        <v>162</v>
+      </c>
+      <c r="J37">
+        <v>11.1</v>
+      </c>
+      <c r="K37">
+        <v>39.96</v>
+      </c>
+      <c r="L37">
+        <v>-123.3</v>
+      </c>
+      <c r="M37">
+        <v>49.28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>662</v>
+      </c>
+      <c r="B38">
+        <v>813.1</v>
+      </c>
+      <c r="C38">
+        <v>1752</v>
+      </c>
+      <c r="D38">
+        <v>-3.94999999999999</v>
+      </c>
+      <c r="E38">
+        <v>-8.25</v>
+      </c>
+      <c r="F38">
+        <v>72</v>
+      </c>
+      <c r="G38">
+        <v>6.86</v>
+      </c>
+      <c r="H38">
+        <v>-6.06</v>
+      </c>
+      <c r="I38">
+        <v>139</v>
+      </c>
+      <c r="J38">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K38">
+        <v>33.119999999999997</v>
+      </c>
+      <c r="L38">
+        <v>-123.29</v>
+      </c>
+      <c r="M38">
+        <v>49.27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>999.8</v>
+      </c>
+      <c r="C39">
+        <v>88</v>
+      </c>
+      <c r="D39">
+        <v>6.0500000000000096</v>
+      </c>
+      <c r="E39">
+        <v>2.8500000000000201</v>
+      </c>
+      <c r="F39">
+        <v>80</v>
+      </c>
+      <c r="G39">
+        <v>-12.34</v>
+      </c>
+      <c r="H39">
+        <v>-0.43</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>12.3</v>
+      </c>
+      <c r="K39">
+        <v>44.28</v>
+      </c>
+      <c r="L39">
+        <v>-123.24</v>
+      </c>
+      <c r="M39">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>998.3</v>
+      </c>
+      <c r="C40">
+        <v>100</v>
+      </c>
+      <c r="D40">
+        <v>4.8500000000000201</v>
+      </c>
+      <c r="E40">
+        <v>-1.25</v>
+      </c>
+      <c r="F40">
+        <v>64</v>
+      </c>
+      <c r="G40">
+        <v>1.56</v>
+      </c>
+      <c r="H40">
+        <v>1.38</v>
+      </c>
+      <c r="I40">
+        <v>221</v>
+      </c>
+      <c r="J40">
+        <v>2.1</v>
+      </c>
+      <c r="K40">
+        <v>7.56</v>
+      </c>
+      <c r="L40">
+        <v>-123.24</v>
+      </c>
+      <c r="M40">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>88</v>
+      </c>
+      <c r="B41">
+        <v>970.7</v>
+      </c>
+      <c r="C41">
+        <v>329</v>
+      </c>
+      <c r="D41">
+        <v>4.3500000000000201</v>
+      </c>
+      <c r="E41">
+        <v>-0.849999999999966</v>
+      </c>
+      <c r="F41">
+        <v>69</v>
+      </c>
+      <c r="G41">
+        <v>-0.11</v>
+      </c>
+      <c r="H41">
+        <v>-0.47</v>
+      </c>
+      <c r="I41">
+        <v>360</v>
+      </c>
+      <c r="J41">
+        <v>0.5</v>
+      </c>
+      <c r="K41">
+        <v>1.8</v>
+      </c>
+      <c r="L41">
+        <v>-123.24</v>
+      </c>
+      <c r="M41">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>140</v>
+      </c>
+      <c r="B42">
+        <v>951.4</v>
+      </c>
+      <c r="C42">
+        <v>492</v>
+      </c>
+      <c r="D42">
+        <v>3.6500000000000301</v>
+      </c>
+      <c r="E42">
+        <v>-2.3499999999999699</v>
+      </c>
+      <c r="F42">
+        <v>65</v>
+      </c>
+      <c r="G42">
+        <v>-1.18</v>
+      </c>
+      <c r="H42">
+        <v>-3.68</v>
+      </c>
+      <c r="I42">
+        <v>72</v>
+      </c>
+      <c r="J42">
+        <v>3.9</v>
+      </c>
+      <c r="K42">
+        <v>14.04</v>
+      </c>
+      <c r="L42">
+        <v>-123.24</v>
+      </c>
+      <c r="M42">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>178</v>
+      </c>
+      <c r="B43">
+        <v>942</v>
+      </c>
+      <c r="C43">
+        <v>573</v>
+      </c>
+      <c r="D43">
+        <v>4.8500000000000201</v>
+      </c>
+      <c r="E43">
+        <v>-8.25</v>
+      </c>
+      <c r="F43">
+        <v>38</v>
+      </c>
+      <c r="G43">
+        <v>-0.69</v>
+      </c>
+      <c r="H43">
+        <v>-5.18</v>
+      </c>
+      <c r="I43">
+        <v>82</v>
+      </c>
+      <c r="J43">
+        <v>5.2</v>
+      </c>
+      <c r="K43">
+        <v>18.72</v>
+      </c>
+      <c r="L43">
+        <v>-123.24</v>
+      </c>
+      <c r="M43">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>394</v>
+      </c>
+      <c r="B44">
+        <v>875</v>
+      </c>
+      <c r="C44">
+        <v>1170</v>
+      </c>
+      <c r="D44">
+        <v>0.25</v>
+      </c>
+      <c r="E44">
+        <v>-13.65</v>
+      </c>
+      <c r="F44">
+        <v>34</v>
+      </c>
+      <c r="G44">
+        <v>3.16</v>
+      </c>
+      <c r="H44">
+        <v>-7.91</v>
+      </c>
+      <c r="I44">
+        <v>112</v>
+      </c>
+      <c r="J44">
+        <v>8.5</v>
+      </c>
+      <c r="K44">
+        <v>30.6</v>
+      </c>
+      <c r="L44">
+        <v>-123.27</v>
+      </c>
+      <c r="M44">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>632</v>
+      </c>
+      <c r="B45">
+        <v>819.2</v>
+      </c>
+      <c r="C45">
+        <v>1693</v>
+      </c>
+      <c r="D45">
+        <v>-3.5499999999999501</v>
+      </c>
+      <c r="E45">
+        <v>-9.8499999999999694</v>
+      </c>
+      <c r="F45">
+        <v>62</v>
+      </c>
+      <c r="G45">
+        <v>6.92</v>
+      </c>
+      <c r="H45">
+        <v>-6.11</v>
+      </c>
+      <c r="I45">
+        <v>139</v>
+      </c>
+      <c r="J45">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K45">
+        <v>33.119999999999997</v>
+      </c>
+      <c r="L45">
+        <v>-123.29</v>
+      </c>
+      <c r="M45">
+        <v>49.26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>530</v>
+      </c>
+      <c r="B46">
+        <v>842.4</v>
+      </c>
+      <c r="C46">
+        <v>1472</v>
+      </c>
+      <c r="D46">
+        <v>-2.1499999999999799</v>
+      </c>
+      <c r="E46">
+        <v>-9.3499999999999694</v>
+      </c>
+      <c r="F46">
+        <v>58</v>
+      </c>
+      <c r="G46">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="H46">
+        <v>-6.92</v>
+      </c>
+      <c r="I46">
+        <v>125</v>
+      </c>
+      <c r="J46">
+        <v>8.5</v>
+      </c>
+      <c r="K46">
+        <v>30.6</v>
+      </c>
+      <c r="L46">
+        <v>-123.28</v>
+      </c>
+      <c r="M46">
+        <v>49.26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K59" t="s">
+        <v>16</v>
+      </c>
+      <c r="L59" t="s">
+        <v>17</v>
+      </c>
+      <c r="M59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>999.8</v>
+      </c>
+      <c r="C60">
+        <v>88</v>
+      </c>
+      <c r="D60">
+        <v>6.0500000000000096</v>
+      </c>
+      <c r="E60">
+        <v>2.8500000000000201</v>
+      </c>
+      <c r="F60">
+        <v>80</v>
+      </c>
+      <c r="G60">
+        <v>-12.34</v>
+      </c>
+      <c r="H60">
+        <v>-0.43</v>
+      </c>
+      <c r="I60">
+        <v>2</v>
+      </c>
+      <c r="J60">
+        <v>12.3</v>
+      </c>
+      <c r="K60">
+        <v>44.28</v>
+      </c>
+      <c r="L60">
+        <v>-123.24</v>
+      </c>
+      <c r="M60">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>14</v>
+      </c>
+      <c r="B61">
+        <v>995.7</v>
+      </c>
+      <c r="C61">
+        <v>121</v>
+      </c>
+      <c r="D61">
+        <v>5.0500000000000096</v>
+      </c>
+      <c r="E61">
+        <v>-0.75</v>
+      </c>
+      <c r="F61">
+        <v>66</v>
+      </c>
+      <c r="G61">
+        <v>2.17</v>
+      </c>
+      <c r="H61">
+        <v>2.39</v>
+      </c>
+      <c r="I61">
+        <v>228</v>
+      </c>
+      <c r="J61">
+        <v>3.2</v>
+      </c>
+      <c r="K61">
+        <v>11.52</v>
+      </c>
+      <c r="L61">
+        <v>-123.24</v>
+      </c>
+      <c r="M61">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>138</v>
+      </c>
+      <c r="B62">
+        <v>951.8</v>
+      </c>
+      <c r="C62">
+        <v>489</v>
+      </c>
+      <c r="D62">
+        <v>3.6500000000000301</v>
+      </c>
+      <c r="E62">
+        <v>-2.3499999999999699</v>
+      </c>
+      <c r="F62">
+        <v>64</v>
+      </c>
+      <c r="G62">
+        <v>-1.21</v>
+      </c>
+      <c r="H62">
+        <v>-3.51</v>
+      </c>
+      <c r="I62">
+        <v>71</v>
+      </c>
+      <c r="J62">
+        <v>3.7</v>
+      </c>
+      <c r="K62">
+        <v>13.32</v>
+      </c>
+      <c r="L62">
+        <v>-123.24</v>
+      </c>
+      <c r="M62">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>160</v>
+      </c>
+      <c r="B63">
+        <v>947</v>
+      </c>
+      <c r="C63">
+        <v>530</v>
+      </c>
+      <c r="D63">
+        <v>5.1500000000000297</v>
+      </c>
+      <c r="E63">
+        <v>-7.25</v>
+      </c>
+      <c r="F63">
+        <v>40</v>
+      </c>
+      <c r="G63">
+        <v>-0.99</v>
+      </c>
+      <c r="H63">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="I63">
+        <v>78</v>
+      </c>
+      <c r="J63">
+        <v>4.7</v>
+      </c>
+      <c r="K63">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="L63">
+        <v>-123.24</v>
+      </c>
+      <c r="M63">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>2164</v>
+      </c>
+      <c r="B64">
+        <v>531.20000000000005</v>
+      </c>
+      <c r="C64">
+        <v>4972</v>
+      </c>
+      <c r="D64">
+        <v>-27.85</v>
+      </c>
+      <c r="E64">
+        <v>-29.95</v>
+      </c>
+      <c r="F64">
+        <v>82</v>
+      </c>
+      <c r="G64">
+        <v>7.7</v>
+      </c>
+      <c r="H64">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="I64">
+        <v>231</v>
+      </c>
+      <c r="J64">
+        <v>12.3</v>
+      </c>
+      <c r="K64">
+        <v>44.28</v>
+      </c>
+      <c r="L64">
+        <v>-123.25</v>
+      </c>
+      <c r="M64">
+        <v>49.37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>2316</v>
+      </c>
+      <c r="B65">
+        <v>507.7</v>
+      </c>
+      <c r="C65">
+        <v>5296</v>
+      </c>
+      <c r="D65">
+        <v>-27.85</v>
+      </c>
+      <c r="E65">
+        <v>-52.35</v>
+      </c>
+      <c r="F65">
+        <v>8</v>
+      </c>
+      <c r="G65">
+        <v>4.79</v>
+      </c>
+      <c r="H65">
+        <v>6.1</v>
+      </c>
+      <c r="I65">
+        <v>232</v>
+      </c>
+      <c r="J65">
+        <v>7.8</v>
+      </c>
+      <c r="K65">
+        <v>28.08</v>
+      </c>
+      <c r="L65">
+        <v>-123.24</v>
+      </c>
+      <c r="M65">
+        <v>49.38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>4776</v>
+      </c>
+      <c r="B66">
+        <v>219.8</v>
+      </c>
+      <c r="C66">
+        <v>10862</v>
+      </c>
+      <c r="D66">
+        <v>-50.25</v>
+      </c>
+      <c r="E66">
+        <v>-82.25</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>7.2</v>
+      </c>
+      <c r="H66">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I66">
+        <v>184</v>
+      </c>
+      <c r="J66">
+        <v>7.2</v>
+      </c>
+      <c r="K66">
+        <v>25.92</v>
+      </c>
+      <c r="L66">
+        <v>-123.12</v>
+      </c>
+      <c r="M66">
+        <v>49.57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>4146</v>
+      </c>
+      <c r="B67">
+        <v>276.8</v>
+      </c>
+      <c r="C67">
+        <v>9379</v>
+      </c>
+      <c r="D67">
+        <v>-55.25</v>
+      </c>
+      <c r="E67">
+        <v>-69.349999999999994</v>
+      </c>
+      <c r="F67">
+        <v>16</v>
+      </c>
+      <c r="G67">
+        <v>9.86</v>
+      </c>
+      <c r="H67">
+        <v>6.97</v>
+      </c>
+      <c r="I67">
+        <v>215</v>
+      </c>
+      <c r="J67">
+        <v>12.1</v>
+      </c>
+      <c r="K67">
+        <v>43.56</v>
+      </c>
+      <c r="L67">
+        <v>-123.13</v>
+      </c>
+      <c r="M67">
+        <v>49.51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>5778</v>
+      </c>
+      <c r="B68">
+        <v>151.4</v>
+      </c>
+      <c r="C68">
+        <v>13305</v>
+      </c>
+      <c r="D68">
+        <v>-48.25</v>
+      </c>
+      <c r="E68">
+        <v>-82.55</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>8.65</v>
+      </c>
+      <c r="H68">
+        <v>2.73</v>
+      </c>
+      <c r="I68">
+        <v>198</v>
+      </c>
+      <c r="J68">
+        <v>9.1</v>
+      </c>
+      <c r="K68">
+        <v>32.76</v>
+      </c>
+      <c r="L68">
+        <v>-123.1</v>
+      </c>
+      <c r="M68">
+        <v>49.64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>6178</v>
+      </c>
+      <c r="B69">
+        <v>128.69999999999999</v>
+      </c>
+      <c r="C69">
+        <v>14366</v>
+      </c>
+      <c r="D69">
+        <v>-51.65</v>
+      </c>
+      <c r="E69">
+        <v>-84.95</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="H69">
+        <v>1.73</v>
+      </c>
+      <c r="I69">
+        <v>191</v>
+      </c>
+      <c r="J69">
+        <v>8.9</v>
+      </c>
+      <c r="K69">
+        <v>32.04</v>
+      </c>
+      <c r="L69">
+        <v>-123.09</v>
+      </c>
+      <c r="M69">
+        <v>49.66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>6938</v>
+      </c>
+      <c r="B70">
+        <v>94.8</v>
+      </c>
+      <c r="C70">
+        <v>16355</v>
+      </c>
+      <c r="D70">
+        <v>-50.35</v>
+      </c>
+      <c r="E70">
+        <v>-84.05</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>10.74</v>
+      </c>
+      <c r="H70">
+        <v>3.57</v>
+      </c>
+      <c r="I70">
+        <v>198</v>
+      </c>
+      <c r="J70">
+        <v>11.3</v>
+      </c>
+      <c r="K70">
+        <v>40.68</v>
+      </c>
+      <c r="L70">
+        <v>-123.06</v>
+      </c>
+      <c r="M70">
+        <v>49.71</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>7590</v>
+      </c>
+      <c r="B71">
+        <v>72.2</v>
+      </c>
+      <c r="C71">
+        <v>18115</v>
+      </c>
+      <c r="D71">
         <v>-54.45</v>
       </c>
-      <c r="E28">
-        <v>-71.650000000000006</v>
-      </c>
-      <c r="F28">
-        <v>11</v>
-      </c>
-      <c r="G28">
-        <v>10.89</v>
-      </c>
-      <c r="H28">
-        <v>8.91</v>
-      </c>
-      <c r="I28">
-        <v>219</v>
-      </c>
-      <c r="J28">
-        <v>14.1</v>
-      </c>
-      <c r="K28">
-        <v>50.76</v>
-      </c>
-      <c r="L28">
-        <v>-123.15</v>
-      </c>
-      <c r="M28">
-        <v>49.5</v>
+      <c r="E71">
+        <v>-86.85</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>6.8</v>
+      </c>
+      <c r="H71">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I71">
+        <v>190</v>
+      </c>
+      <c r="J71">
+        <v>6.9</v>
+      </c>
+      <c r="K71">
+        <v>24.84</v>
+      </c>
+      <c r="L71">
+        <v>-123.03</v>
+      </c>
+      <c r="M71">
+        <v>49.74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>8318</v>
+      </c>
+      <c r="B72">
+        <v>53.7</v>
+      </c>
+      <c r="C72">
+        <v>20027</v>
+      </c>
+      <c r="D72">
+        <v>-50.05</v>
+      </c>
+      <c r="E72">
+        <v>-83.85</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>2.42</v>
+      </c>
+      <c r="H72">
+        <v>-3.31</v>
+      </c>
+      <c r="I72">
+        <v>126</v>
+      </c>
+      <c r="J72">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K72">
+        <v>14.76</v>
+      </c>
+      <c r="L72">
+        <v>-123.01</v>
+      </c>
+      <c r="M72">
+        <v>49.76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>8584</v>
+      </c>
+      <c r="B73">
+        <v>47.9</v>
+      </c>
+      <c r="C73">
+        <v>20763</v>
+      </c>
+      <c r="D73">
+        <v>-52.15</v>
+      </c>
+      <c r="E73">
+        <v>-85.25</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>3.25</v>
+      </c>
+      <c r="H73">
+        <v>-6.21</v>
+      </c>
+      <c r="I73">
+        <v>118</v>
+      </c>
+      <c r="J73">
+        <v>7</v>
+      </c>
+      <c r="K73">
+        <v>25.2</v>
+      </c>
+      <c r="L73">
+        <v>-123.02</v>
+      </c>
+      <c r="M73">
+        <v>49.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>